<commit_message>
Se cambia clase Invoice to Api. Lógica para Factura o remision.
</commit_message>
<xml_diff>
--- a/data - copia.xlsx
+++ b/data - copia.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pendientes" sheetId="1" state="visible" r:id="rId1"/>
@@ -474,7 +474,7 @@
       </c>
       <c r="C1" s="30" t="inlineStr">
         <is>
-          <t>FACT / REMIS</t>
+          <t>FACT/REMIS</t>
         </is>
       </c>
       <c r="D1" s="30" t="inlineStr">
@@ -605,7 +605,7 @@
       </c>
       <c r="C1" s="30" t="inlineStr">
         <is>
-          <t>FACT / REMIS</t>
+          <t>FACT/REMIS</t>
         </is>
       </c>
       <c r="D1" s="30" t="inlineStr">

</xml_diff>

<commit_message>
Se obtiene id del cliente a través del DNI.
</commit_message>
<xml_diff>
--- a/data - copia.xlsx
+++ b/data - copia.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pendientes" sheetId="1" state="visible" r:id="rId1"/>
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,85 +489,90 @@
       </c>
       <c r="F1" s="30" t="inlineStr">
         <is>
+          <t>ClienteDNI</t>
+        </is>
+      </c>
+      <c r="G1" s="30" t="inlineStr">
+        <is>
           <t>Cliente</t>
         </is>
       </c>
-      <c r="G1" s="30" t="inlineStr">
+      <c r="H1" s="30" t="inlineStr">
         <is>
           <t>Población</t>
         </is>
       </c>
-      <c r="H1" s="30" t="inlineStr">
+      <c r="I1" s="30" t="inlineStr">
         <is>
           <t>FAC/REM</t>
         </is>
       </c>
-      <c r="I1" s="30" t="inlineStr">
+      <c r="J1" s="30" t="inlineStr">
         <is>
           <t>Transportadora</t>
         </is>
       </c>
-      <c r="J1" s="30" t="inlineStr">
+      <c r="K1" s="30" t="inlineStr">
         <is>
           <t>Guía</t>
         </is>
       </c>
-      <c r="K1" s="30" t="inlineStr">
+      <c r="L1" s="30" t="inlineStr">
         <is>
           <t>#Paquetes</t>
         </is>
       </c>
-      <c r="L1" s="30" t="inlineStr">
+      <c r="M1" s="30" t="inlineStr">
         <is>
           <t>Empacó</t>
         </is>
       </c>
-      <c r="M1" s="30" t="inlineStr">
+      <c r="N1" s="30" t="inlineStr">
         <is>
           <t>NOTAS</t>
         </is>
       </c>
-      <c r="N1" s="30" t="inlineStr">
+      <c r="O1" s="30" t="inlineStr">
         <is>
           <t>Referencia</t>
         </is>
       </c>
-      <c r="O1" s="30" t="inlineStr">
+      <c r="P1" s="30" t="inlineStr">
         <is>
           <t>Articulo</t>
         </is>
       </c>
-      <c r="P1" s="30" t="inlineStr">
+      <c r="Q1" s="30" t="inlineStr">
         <is>
           <t>Cantidad</t>
         </is>
       </c>
-      <c r="Q1" s="30" t="inlineStr">
+      <c r="R1" s="30" t="inlineStr">
         <is>
           <t>Precio</t>
         </is>
       </c>
-      <c r="R1" s="30" t="inlineStr">
+      <c r="S1" s="30" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="S1" s="30" t="inlineStr">
+      <c r="T1" s="30" t="inlineStr">
         <is>
           <t>Peso (kg)</t>
         </is>
       </c>
-      <c r="T1" s="30" t="inlineStr">
+      <c r="U1" s="30" t="inlineStr">
         <is>
           <t># paquetes</t>
         </is>
       </c>
-      <c r="U1" s="30" t="inlineStr">
+      <c r="V1" s="30" t="inlineStr">
         <is>
           <t>Precios  IVA incl</t>
         </is>
       </c>
-      <c r="V1" s="30" t="inlineStr">
+      <c r="W1" s="30" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -584,7 +589,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -620,85 +625,90 @@
       </c>
       <c r="F1" s="30" t="inlineStr">
         <is>
+          <t>ClienteDNI</t>
+        </is>
+      </c>
+      <c r="G1" s="30" t="inlineStr">
+        <is>
           <t>Cliente</t>
         </is>
       </c>
-      <c r="G1" s="30" t="inlineStr">
+      <c r="H1" s="30" t="inlineStr">
         <is>
           <t>Población</t>
         </is>
       </c>
-      <c r="H1" s="30" t="inlineStr">
+      <c r="I1" s="30" t="inlineStr">
         <is>
           <t>FAC/REM</t>
         </is>
       </c>
-      <c r="I1" s="30" t="inlineStr">
+      <c r="J1" s="30" t="inlineStr">
         <is>
           <t>Transportadora</t>
         </is>
       </c>
-      <c r="J1" s="30" t="inlineStr">
+      <c r="K1" s="30" t="inlineStr">
         <is>
           <t>Guía</t>
         </is>
       </c>
-      <c r="K1" s="30" t="inlineStr">
+      <c r="L1" s="30" t="inlineStr">
         <is>
           <t>#Paquetes</t>
         </is>
       </c>
-      <c r="L1" s="30" t="inlineStr">
+      <c r="M1" s="30" t="inlineStr">
         <is>
           <t>Empacó</t>
         </is>
       </c>
-      <c r="M1" s="30" t="inlineStr">
+      <c r="N1" s="30" t="inlineStr">
         <is>
           <t>NOTAS</t>
         </is>
       </c>
-      <c r="N1" s="30" t="inlineStr">
+      <c r="O1" s="30" t="inlineStr">
         <is>
           <t>Referencia</t>
         </is>
       </c>
-      <c r="O1" s="30" t="inlineStr">
+      <c r="P1" s="30" t="inlineStr">
         <is>
           <t>Articulo</t>
         </is>
       </c>
-      <c r="P1" s="30" t="inlineStr">
+      <c r="Q1" s="30" t="inlineStr">
         <is>
           <t>Cantidad</t>
         </is>
       </c>
-      <c r="Q1" s="30" t="inlineStr">
+      <c r="R1" s="30" t="inlineStr">
         <is>
           <t>Precio</t>
         </is>
       </c>
-      <c r="R1" s="30" t="inlineStr">
+      <c r="S1" s="30" t="inlineStr">
         <is>
           <t>Subtotal</t>
         </is>
       </c>
-      <c r="S1" s="30" t="inlineStr">
+      <c r="T1" s="30" t="inlineStr">
         <is>
           <t>Peso (kg)</t>
         </is>
       </c>
-      <c r="T1" s="30" t="inlineStr">
+      <c r="U1" s="30" t="inlineStr">
         <is>
           <t># paquetes</t>
         </is>
       </c>
-      <c r="U1" s="30" t="inlineStr">
+      <c r="V1" s="30" t="inlineStr">
         <is>
           <t>Precios  IVA incl</t>
         </is>
       </c>
-      <c r="V1" s="30" t="inlineStr">
+      <c r="W1" s="30" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -722,55 +732,58 @@
         </is>
       </c>
       <c r="F2" t="n">
+        <v>12345</v>
+      </c>
+      <c r="G2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Armenia</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Estelar Express</t>
         </is>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>14228</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>1</v>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Luis Rendón</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>5 pacas</t>
         </is>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>1</v>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>Fibra pp 12000 200 gr surtida</t>
         </is>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>180</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>1791</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>322380</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>36</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -795,118 +808,53 @@
         <v>0.19</v>
       </c>
       <c r="F3" t="n">
+        <v>12345</v>
+      </c>
+      <c r="G3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Tuluá</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Estelar Express</t>
         </is>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>15751</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>1</v>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Luis Rendón</t>
         </is>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>1</v>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>Soga cabuya 1/2 13mm 204m</t>
         </is>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>204</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>1280</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>261120</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>25</v>
       </c>
-      <c r="U3" t="n">
-        <v>1523.2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="32" t="n">
-        <v>44365</v>
-      </c>
-      <c r="B4" t="n">
-        <v>30</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Facturado</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Tuluá</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Estelar Express</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
-        <v>15751</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Luis Rendón</t>
-        </is>
-      </c>
-      <c r="N4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Soga cabuya 1/2 13mm 204m</t>
-        </is>
-      </c>
-      <c r="P4" t="n">
-        <v>204</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>1280</v>
-      </c>
-      <c r="R4" t="n">
-        <v>261120</v>
-      </c>
-      <c r="S4" t="n">
-        <v>25</v>
-      </c>
-      <c r="U4" t="n">
+      <c r="V3" t="n">
         <v>1523.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se obtiene id del producto a través del nombre, se adjunta a factura y remision.
</commit_message>
<xml_diff>
--- a/data - copia.xlsx
+++ b/data - copia.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pendientes" sheetId="1" state="visible" r:id="rId1"/>
@@ -734,8 +734,10 @@
       <c r="F2" t="n">
         <v>12345</v>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Pedrito</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -763,8 +765,10 @@
           <t>5 pacas</t>
         </is>
       </c>
-      <c r="O2" t="n">
-        <v>1</v>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Clavos 100gr</t>
+        </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -775,10 +779,10 @@
         <v>180</v>
       </c>
       <c r="R2" t="n">
-        <v>1791</v>
+        <v>2000</v>
       </c>
       <c r="S2" t="n">
-        <v>322380</v>
+        <v>360000</v>
       </c>
       <c r="T2" t="n">
         <v>36</v>
@@ -810,8 +814,10 @@
       <c r="F3" t="n">
         <v>12345</v>
       </c>
-      <c r="G3" t="n">
-        <v>1</v>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Juanito</t>
+        </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -834,8 +840,10 @@
           <t>Luis Rendón</t>
         </is>
       </c>
-      <c r="O3" t="n">
-        <v>1</v>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Clavos 200gr</t>
+        </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -846,10 +854,10 @@
         <v>204</v>
       </c>
       <c r="R3" t="n">
-        <v>1280</v>
+        <v>3000</v>
       </c>
       <c r="S3" t="n">
-        <v>261120</v>
+        <v>612000</v>
       </c>
       <c r="T3" t="n">
         <v>25</v>

</xml_diff>

<commit_message>
Se ajustan envio de facturas y remisiones.
</commit_message>
<xml_diff>
--- a/data - copia.xlsx
+++ b/data - copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marif\Desktop\alegraApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A18020-024B-45AC-A7A9-46EAD3A22A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D447590-022E-4AF5-A75B-BD61A7497F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>Cliente</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>698</t>
+  </si>
+  <si>
+    <t>Super Expres</t>
   </si>
 </sst>
 </file>
@@ -470,8 +473,8 @@
   </sheetPr>
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -552,7 +555,7 @@
         <v>44366</v>
       </c>
       <c r="B2" s="8">
-        <v>44731</v>
+        <v>44732</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="9" t="s">
@@ -573,7 +576,9 @@
       <c r="I2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="9"/>
+      <c r="J2" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="K2" s="9">
         <v>4567</v>
       </c>
@@ -613,7 +618,7 @@
         <v>44365</v>
       </c>
       <c r="B3" s="8">
-        <v>44732</v>
+        <v>44731</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="9" t="s">

</xml_diff>